<commit_message>
fix: demo books authors
</commit_message>
<xml_diff>
--- a/books.xlsx
+++ b/books.xlsx
@@ -256,7 +256,7 @@
     <t xml:space="preserve">Communication Studies</t>
   </si>
   <si>
-    <t xml:space="preserve">Mia Moody-Ramirez-Hazel James Cole</t>
+    <t xml:space="preserve">Mia Moody-Ramirez; Hazel James Cole</t>
   </si>
   <si>
     <t xml:space="preserve">Race, Gender, and Image Repair Theory : How Digital Media Change the Landscape</t>
@@ -331,7 +331,7 @@
     <t xml:space="preserve">956.04</t>
   </si>
   <si>
-    <t xml:space="preserve">Alice Vittrant-Justin Watkins</t>
+    <t xml:space="preserve">Alice Vittrant; Justin Watkins</t>
   </si>
   <si>
     <t xml:space="preserve">The Mainland Southeast Asia Linguistic Area</t>
@@ -481,7 +481,7 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView showFormulas="true" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
add: number of pages
</commit_message>
<xml_diff>
--- a/books.xlsx
+++ b/books.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="111">
   <si>
     <t xml:space="preserve">bisac</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t xml:space="preserve">format</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pages</t>
   </si>
   <si>
     <t xml:space="preserve">MATHEMATICS</t>
@@ -359,11 +362,11 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -381,13 +384,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -417,7 +413,7 @@
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
@@ -440,25 +436,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -478,513 +462,545 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView showFormulas="true" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="7.89453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="23.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="10.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="34.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="68.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="23.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="19.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="20.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="26.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="10.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="11.99"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="15" style="1" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="10.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="51.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="21.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="24.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="9.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="10.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="10.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="3" t="n">
+      <c r="C2" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="0" t="n">
         <v>2019</v>
       </c>
-      <c r="E2" s="4" t="n">
+      <c r="E2" s="0" t="n">
         <v>1857555</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="4" t="s">
+      <c r="I2" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="J2" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="K2" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="L2" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="M2" s="0" t="s">
         <v>24</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" s="0" t="n">
+        <v>272</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="3" t="n">
+      <c r="C3" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="0" t="n">
         <v>2022</v>
       </c>
-      <c r="E3" s="4" t="n">
+      <c r="E3" s="0" t="n">
         <v>3241753</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="3" t="s">
+      <c r="F3" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="G3" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="H3" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="I3" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="J3" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="K3" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="L3" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="M3" s="0" t="s">
         <v>36</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="O3" s="0" t="n">
+        <v>465</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>2018</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>1819683</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="N4" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" s="3" t="n">
-        <v>2018</v>
-      </c>
-      <c r="E4" s="4" t="n">
-        <v>1819683</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>36</v>
+      <c r="O4" s="0" t="n">
+        <v>298</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>2246475</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="M5" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="N5" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="3" t="n">
-        <v>2019</v>
-      </c>
-      <c r="E5" s="4" t="n">
-        <v>2246475</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="N5" s="4" t="s">
-        <v>36</v>
+      <c r="O5" s="0" t="n">
+        <v>312</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B6" s="3" t="s">
+      <c r="A6" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="B6" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="D6" s="3" t="n">
+      <c r="C6" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="0" t="n">
         <v>2014</v>
       </c>
-      <c r="E6" s="4" t="n">
+      <c r="E6" s="0" t="n">
         <v>676913</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="G6" s="3" t="s">
+      <c r="F6" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="G6" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="H6" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="I6" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="J6" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="L6" s="4" t="s">
+      <c r="K6" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="M6" s="4" t="s">
+      <c r="L6" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="N6" s="4" t="s">
-        <v>36</v>
+      <c r="M6" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="N6" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="O6" s="0" t="n">
+        <v>316</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B7" s="3" t="s">
+      <c r="A7" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="B7" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="D7" s="3" t="n">
+      <c r="C7" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="0" t="n">
         <v>2016</v>
       </c>
-      <c r="E7" s="4" t="n">
+      <c r="E7" s="0" t="n">
         <v>1081010</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G7" s="3" t="s">
+      <c r="F7" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="G7" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="H7" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="I7" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="J7" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="K7" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="M7" s="4" t="s">
+      <c r="L7" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="N7" s="4" t="s">
-        <v>36</v>
+      <c r="M7" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="N7" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="O7" s="0" t="n">
+        <v>382</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
+    <row r="8" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>2018</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>1947642</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="K8" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="L8" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="M8" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="N8" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="3" t="n">
-        <v>2018</v>
-      </c>
-      <c r="E8" s="4" t="n">
-        <v>1947642</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="M8" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="N8" s="4" t="s">
-        <v>36</v>
+      <c r="O8" s="0" t="n">
+        <v>251</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>2894802</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="K9" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="L9" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="M9" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="N9" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D9" s="3" t="n">
-        <v>2021</v>
-      </c>
-      <c r="E9" s="4" t="n">
-        <v>2894802</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="K9" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="M9" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="N9" s="4" t="s">
-        <v>24</v>
+      <c r="O9" s="0" t="n">
+        <v>272</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B10" s="3" t="s">
+      <c r="A10" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="3" t="n">
+      <c r="B10" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="0" t="n">
         <v>2018</v>
       </c>
-      <c r="E10" s="4" t="n">
+      <c r="E10" s="0" t="n">
         <v>1891782</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="G10" s="3" t="s">
+      <c r="F10" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="H10" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I10" s="4" t="s">
+      <c r="G10" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="H10" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="I10" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="K10" s="4" t="s">
+      <c r="J10" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="L10" s="4" t="s">
+      <c r="K10" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="M10" s="4" t="s">
+      <c r="L10" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="N10" s="4" t="s">
-        <v>36</v>
+      <c r="M10" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="N10" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="O10" s="0" t="n">
+        <v>234</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>2157092</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="K11" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="L11" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="M11" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="N11" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="3" t="n">
-        <v>2019</v>
-      </c>
-      <c r="E11" s="4" t="n">
-        <v>2157092</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="L11" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="M11" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="N11" s="4" t="s">
-        <v>36</v>
+      <c r="O11" s="0" t="n">
+        <v>735</v>
       </c>
     </row>
   </sheetData>

</xml_diff>